<commit_message>
[BUY]  [151021 @ 6.67-151102 @ 6.23][601328 sh.交通银行]-6.597count:  8
</commit_message>
<xml_diff>
--- a/记录.xlsx
+++ b/记录.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="200" windowWidth="25360" windowHeight="14100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="安全资产" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">A!$C$1:$C$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">A!$C$1:$C$42</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="98">
   <si>
     <t>时间</t>
   </si>
@@ -445,6 +445,24 @@
   </si>
   <si>
     <t>清仓。。。没有任何信号，因为恐慌。。这只股票，四个月赚了525</t>
+  </si>
+  <si>
+    <t>27元止损。</t>
+  </si>
+  <si>
+    <t>折腾了一下，投入8k，赚了100块，呵呵</t>
+  </si>
+  <si>
+    <t>151102 @ 6.23]</t>
+  </si>
+  <si>
+    <t>[601328 sh.交通银行]</t>
+  </si>
+  <si>
+    <t>count:  8</t>
+  </si>
+  <si>
+    <t>[BUY]  [151021 @ 6.67 - 151102 @ 6.23] [601328 sh.交通银行] -6.597 count:  8</t>
   </si>
 </sst>
 </file>
@@ -570,8 +588,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="155">
+  <cellStyleXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -792,7 +816,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="155">
+  <cellStyles count="161">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -870,6 +894,9 @@
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -947,6 +974,9 @@
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1276,11 +1306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0"/>
@@ -1322,7 +1351,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>20150518</v>
       </c>
@@ -1345,7 +1374,7 @@
         <v>-2289</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>20150519</v>
       </c>
@@ -1368,7 +1397,7 @@
         <v>-4692</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>20150519</v>
       </c>
@@ -1391,7 +1420,7 @@
         <v>-1539</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>20150601</v>
       </c>
@@ -1414,7 +1443,7 @@
         <v>-7076</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>20150604</v>
       </c>
@@ -1440,7 +1469,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>20150616</v>
       </c>
@@ -1463,7 +1492,7 @@
         <v>-7034</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>20150616</v>
       </c>
@@ -1490,7 +1519,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>20150616</v>
       </c>
@@ -1517,7 +1546,7 @@
       </c>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" hidden="1">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>20150617</v>
       </c>
@@ -1540,7 +1569,7 @@
         <v>-6840</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="7" customFormat="1" ht="63" hidden="1">
+    <row r="11" spans="1:9" s="7" customFormat="1" ht="63">
       <c r="A11" s="7">
         <v>20150617</v>
       </c>
@@ -1589,7 +1618,7 @@
         <v>-8019</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="105" hidden="1">
+    <row r="13" spans="1:9" ht="105">
       <c r="A13" s="7">
         <v>20150626</v>
       </c>
@@ -1616,7 +1645,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1">
+    <row r="14" spans="1:9">
       <c r="A14" s="7">
         <v>20150629</v>
       </c>
@@ -1643,7 +1672,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1">
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>20150703</v>
       </c>
@@ -1692,7 +1721,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1">
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>20150707</v>
       </c>
@@ -1718,7 +1747,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1">
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>20150709</v>
       </c>
@@ -1744,7 +1773,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1">
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>20150710</v>
       </c>
@@ -1770,7 +1799,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1">
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>20150710</v>
       </c>
@@ -1796,7 +1825,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1">
+    <row r="21" spans="1:9">
       <c r="A21" s="7">
         <v>20150710</v>
       </c>
@@ -1823,7 +1852,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1">
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>20150713</v>
       </c>
@@ -1849,7 +1878,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1">
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>20150722</v>
       </c>
@@ -1875,7 +1904,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1">
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>20150727</v>
       </c>
@@ -1901,7 +1930,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1">
+    <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>20150728</v>
       </c>
@@ -1927,7 +1956,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1">
+    <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>20150805</v>
       </c>
@@ -1953,7 +1982,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1">
+    <row r="27" spans="1:9">
       <c r="A27" s="1">
         <v>20150805</v>
       </c>
@@ -2005,7 +2034,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="7" customFormat="1" ht="183" hidden="1" customHeight="1">
+    <row r="29" spans="1:9" s="7" customFormat="1" ht="183" customHeight="1">
       <c r="A29" s="7">
         <v>20150818</v>
       </c>
@@ -2031,7 +2060,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="7" customFormat="1" ht="147" hidden="1">
+    <row r="30" spans="1:9" s="7" customFormat="1" ht="147">
       <c r="A30" s="7">
         <v>20150819</v>
       </c>
@@ -2057,7 +2086,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="7" customFormat="1" ht="147" hidden="1">
+    <row r="31" spans="1:9" s="7" customFormat="1" ht="147">
       <c r="A31" s="7">
         <v>20150820</v>
       </c>
@@ -2083,7 +2112,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1">
+    <row r="32" spans="1:9">
       <c r="A32" s="1">
         <v>20150819</v>
       </c>
@@ -2106,7 +2135,7 @@
         <v>-1253</v>
       </c>
     </row>
-    <row r="33" spans="1:14" hidden="1">
+    <row r="33" spans="1:14">
       <c r="A33" s="1">
         <v>20150821</v>
       </c>
@@ -2132,7 +2161,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="7" customFormat="1" hidden="1">
+    <row r="34" spans="1:14" s="7" customFormat="1">
       <c r="A34" s="7">
         <v>20150825</v>
       </c>
@@ -2158,8 +2187,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:14" hidden="1"/>
-    <row r="36" spans="1:14" s="7" customFormat="1" hidden="1">
+    <row r="36" spans="1:14" s="7" customFormat="1">
       <c r="A36" s="7">
         <v>20150828</v>
       </c>
@@ -2185,7 +2213,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="7" customFormat="1" hidden="1">
+    <row r="37" spans="1:14" s="7" customFormat="1">
       <c r="A37" s="7">
         <v>20150831</v>
       </c>
@@ -2211,7 +2239,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="42" hidden="1">
+    <row r="38" spans="1:14" ht="42">
       <c r="A38" s="1">
         <v>20151008</v>
       </c>
@@ -2231,7 +2259,7 @@
         <v>26.67</v>
       </c>
       <c r="G38" s="1">
-        <v>8002</v>
+        <v>-8002</v>
       </c>
       <c r="I38" s="10" t="s">
         <v>90</v>
@@ -2278,14 +2306,131 @@
         <v>91</v>
       </c>
     </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="1">
+        <v>20151020</v>
+      </c>
+      <c r="B40" s="1">
+        <v>601628</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="1">
+        <v>200</v>
+      </c>
+      <c r="F40" s="1">
+        <v>26.98</v>
+      </c>
+      <c r="G40" s="1">
+        <v>5396</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M40" s="1">
+        <v>-6.9269999999999996</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="1">
+        <v>20151021</v>
+      </c>
+      <c r="B41" s="1">
+        <v>601628</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="1">
+        <v>100</v>
+      </c>
+      <c r="F41" s="1">
+        <v>27.25</v>
+      </c>
+      <c r="G41" s="1">
+        <v>2725</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M41" s="1">
+        <v>-6.9269999999999996</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" s="7" customFormat="1">
+      <c r="A42" s="7">
+        <v>20151103</v>
+      </c>
+      <c r="B42" s="7">
+        <v>601328</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="7">
+        <v>300</v>
+      </c>
+      <c r="F42" s="7">
+        <v>6.19</v>
+      </c>
+      <c r="G42" s="7">
+        <v>-1857</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K42" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="L42" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="M42" s="7">
+        <v>-6.5970000000000004</v>
+      </c>
+      <c r="N42" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="C1:C38">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="中核科技"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="C1:C42"/>
   <mergeCells count="1">
     <mergeCell ref="I8:I9"/>
   </mergeCells>
@@ -2838,7 +2983,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
加米，live to be better
</commit_message>
<xml_diff>
--- a/记录.xlsx
+++ b/记录.xlsx
@@ -16,9 +16,10 @@
     <sheet name="安全资产" sheetId="7" r:id="rId7"/>
     <sheet name="拆借" sheetId="8" r:id="rId8"/>
     <sheet name="纪律" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">A!$C$1:$C$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">A!$C$1:$C$77</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="164">
   <si>
     <t>时间</t>
   </si>
@@ -656,12 +657,65 @@
   <si>
     <t>清仓</t>
   </si>
+  <si>
+    <t>第二波</t>
+  </si>
+  <si>
+    <t>北大荒</t>
+  </si>
+  <si>
+    <t>第一波</t>
+  </si>
+  <si>
+    <t>仓位接近7成。积极止盈</t>
+  </si>
+  <si>
+    <t>致敬！上证50！</t>
+  </si>
+  <si>
+    <t>向上证50致敬之第二次</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[BUY]  [151117 @ 67.88 - 160125 @ 55.00] [002594 sz.比亚迪] -18.975 count: 48
+[BUY]  [151217 @ 63.80 - 160125 @ 55.00] [002594 sz.比亚迪] -13.793 count: 26
+</t>
+  </si>
+  <si>
+    <t>比亚迪</t>
+  </si>
+  <si>
+    <t>0.1W</t>
+  </si>
+  <si>
+    <t>Seq</t>
+  </si>
+  <si>
+    <t>UID</t>
+  </si>
+  <si>
+    <t>176 食堂用户</t>
+  </si>
+  <si>
+    <t>0.45W</t>
+  </si>
+  <si>
+    <t>西部证券</t>
+  </si>
+  <si>
+    <t>满仓了。</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 拆&amp;还</t>
+  </si>
+  <si>
+    <t>僧哥</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -710,6 +764,22 @@
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="Lucida Grande"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Grande"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="Lucida Grande"/>
     </font>
   </fonts>
   <fills count="3">
@@ -789,7 +859,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="223">
+  <cellStyleXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1013,8 +1083,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1112,10 +1219,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1123,11 +1227,43 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="251"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="251"/>
   </cellXfs>
-  <cellStyles count="223">
+  <cellStyles count="260">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1239,6 +1375,28 @@
     <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1350,6 +1508,21 @@
     <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1679,10 +1852,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P66"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0"/>
@@ -1724,7 +1898,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" hidden="1">
       <c r="A2" s="1">
         <v>20150518</v>
       </c>
@@ -1747,7 +1921,7 @@
         <v>-2289</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" hidden="1">
       <c r="A3" s="1">
         <v>20150519</v>
       </c>
@@ -1770,7 +1944,7 @@
         <v>-4692</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" hidden="1">
       <c r="A4" s="1">
         <v>20150519</v>
       </c>
@@ -1793,7 +1967,7 @@
         <v>-1539</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" hidden="1">
       <c r="A5" s="1">
         <v>20150601</v>
       </c>
@@ -1816,7 +1990,7 @@
         <v>-7076</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" hidden="1">
       <c r="A6" s="1">
         <v>20150604</v>
       </c>
@@ -1842,7 +2016,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" hidden="1">
       <c r="A7" s="1">
         <v>20150616</v>
       </c>
@@ -1865,7 +2039,7 @@
         <v>-7034</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" hidden="1">
       <c r="A8" s="1">
         <v>20150616</v>
       </c>
@@ -1888,11 +2062,11 @@
         <v>-6252</v>
       </c>
       <c r="H8" s="9"/>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="48" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" hidden="1">
       <c r="A9" s="1">
         <v>20150616</v>
       </c>
@@ -1917,9 +2091,9 @@
       <c r="H9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="35"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="I9" s="49"/>
+    </row>
+    <row r="10" spans="1:9" hidden="1">
       <c r="A10" s="1">
         <v>20150617</v>
       </c>
@@ -1942,7 +2116,7 @@
         <v>-6840</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="7" customFormat="1" ht="63">
+    <row r="11" spans="1:9" s="7" customFormat="1" ht="63" hidden="1">
       <c r="A11" s="7">
         <v>20150617</v>
       </c>
@@ -1968,7 +2142,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" hidden="1">
       <c r="A12" s="1">
         <v>20150619</v>
       </c>
@@ -1991,7 +2165,7 @@
         <v>-8019</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="105">
+    <row r="13" spans="1:9" ht="105" hidden="1">
       <c r="A13" s="7">
         <v>20150626</v>
       </c>
@@ -2018,7 +2192,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" hidden="1">
       <c r="A14" s="7">
         <v>20150629</v>
       </c>
@@ -2045,7 +2219,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" hidden="1">
       <c r="A15" s="1">
         <v>20150703</v>
       </c>
@@ -2068,7 +2242,7 @@
         <v>-4725</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" hidden="1">
       <c r="A16" s="1">
         <v>20150706</v>
       </c>
@@ -2120,7 +2294,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" hidden="1">
       <c r="A18" s="1">
         <v>20150709</v>
       </c>
@@ -2146,7 +2320,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" hidden="1">
       <c r="A19" s="1">
         <v>20150710</v>
       </c>
@@ -2172,7 +2346,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" hidden="1">
       <c r="A20" s="1">
         <v>20150710</v>
       </c>
@@ -2198,7 +2372,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" hidden="1">
       <c r="A21" s="7">
         <v>20150710</v>
       </c>
@@ -2225,7 +2399,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" hidden="1">
       <c r="A22" s="1">
         <v>20150713</v>
       </c>
@@ -2277,7 +2451,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" hidden="1">
       <c r="A24" s="1">
         <v>20150727</v>
       </c>
@@ -2329,7 +2503,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" hidden="1">
       <c r="A26" s="1">
         <v>20150805</v>
       </c>
@@ -2355,7 +2529,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" hidden="1">
       <c r="A27" s="1">
         <v>20150805</v>
       </c>
@@ -2381,7 +2555,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="7" customFormat="1" ht="42">
+    <row r="28" spans="1:9" s="7" customFormat="1" ht="42" hidden="1">
       <c r="A28" s="7">
         <v>20150810</v>
       </c>
@@ -2407,7 +2581,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="7" customFormat="1" ht="183" customHeight="1">
+    <row r="29" spans="1:9" s="7" customFormat="1" ht="183" hidden="1" customHeight="1">
       <c r="A29" s="7">
         <v>20150818</v>
       </c>
@@ -2433,7 +2607,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="7" customFormat="1" ht="147">
+    <row r="30" spans="1:9" s="7" customFormat="1" ht="147" hidden="1">
       <c r="A30" s="7">
         <v>20150819</v>
       </c>
@@ -2459,7 +2633,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="7" customFormat="1" ht="147">
+    <row r="31" spans="1:9" s="7" customFormat="1" ht="147" hidden="1">
       <c r="A31" s="7">
         <v>20150820</v>
       </c>
@@ -2485,7 +2659,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" hidden="1">
       <c r="A32" s="1">
         <v>20150819</v>
       </c>
@@ -2508,7 +2682,7 @@
         <v>-1253</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="7" customFormat="1">
+    <row r="33" spans="1:16" s="7" customFormat="1" hidden="1">
       <c r="A33" s="7">
         <v>20150825</v>
       </c>
@@ -2534,10 +2708,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" hidden="1">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:16" s="7" customFormat="1">
+    <row r="35" spans="1:16" s="7" customFormat="1" hidden="1">
       <c r="A35" s="7">
         <v>20150828</v>
       </c>
@@ -2563,7 +2737,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="7" customFormat="1">
+    <row r="36" spans="1:16" s="7" customFormat="1" hidden="1">
       <c r="A36" s="7">
         <v>20150831</v>
       </c>
@@ -2589,7 +2763,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="42">
+    <row r="37" spans="1:16" ht="42" hidden="1">
       <c r="A37" s="1">
         <v>20151008</v>
       </c>
@@ -2630,7 +2804,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="7" customFormat="1">
+    <row r="38" spans="1:16" s="7" customFormat="1" hidden="1">
       <c r="A38" s="7">
         <v>20151014</v>
       </c>
@@ -2656,7 +2830,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" hidden="1">
       <c r="A39" s="1">
         <v>20151020</v>
       </c>
@@ -2697,7 +2871,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" hidden="1">
       <c r="A40" s="1">
         <v>20151021</v>
       </c>
@@ -2738,7 +2912,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="7" customFormat="1">
+    <row r="41" spans="1:16" s="7" customFormat="1" hidden="1">
       <c r="A41" s="7">
         <v>20151103</v>
       </c>
@@ -2779,7 +2953,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="42">
+    <row r="42" spans="1:16" ht="42" hidden="1">
       <c r="A42" s="1">
         <v>20151109</v>
       </c>
@@ -2805,7 +2979,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="7" customFormat="1">
+    <row r="43" spans="1:16" s="7" customFormat="1" hidden="1">
       <c r="A43" s="7">
         <v>20151112</v>
       </c>
@@ -2846,7 +3020,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" hidden="1">
       <c r="A44" s="1">
         <v>20151201</v>
       </c>
@@ -2887,7 +3061,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="7" customFormat="1" ht="63">
+    <row r="45" spans="1:16" s="7" customFormat="1" ht="63" hidden="1">
       <c r="A45" s="7">
         <v>20151202</v>
       </c>
@@ -2913,7 +3087,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="42">
+    <row r="46" spans="1:16" ht="42" hidden="1">
       <c r="A46" s="1">
         <v>20151204</v>
       </c>
@@ -2954,7 +3128,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="7" customFormat="1">
+    <row r="47" spans="1:16" s="7" customFormat="1" hidden="1">
       <c r="A47" s="7">
         <v>20151204</v>
       </c>
@@ -2978,7 +3152,7 @@
       </c>
       <c r="I47" s="22"/>
     </row>
-    <row r="48" spans="1:16" s="7" customFormat="1" ht="42">
+    <row r="48" spans="1:16" s="7" customFormat="1" ht="42" hidden="1">
       <c r="A48" s="7">
         <v>20151211</v>
       </c>
@@ -3003,16 +3177,16 @@
       <c r="I48" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="K48" s="36" t="s">
+      <c r="K48" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="L48" s="37"/>
-      <c r="M48" s="37"/>
-      <c r="N48" s="37"/>
-      <c r="O48" s="37"/>
-      <c r="P48" s="37"/>
-    </row>
-    <row r="49" spans="1:16">
+      <c r="L48" s="47"/>
+      <c r="M48" s="47"/>
+      <c r="N48" s="47"/>
+      <c r="O48" s="47"/>
+      <c r="P48" s="47"/>
+    </row>
+    <row r="49" spans="1:16" hidden="1">
       <c r="A49" s="23">
         <v>20151211</v>
       </c>
@@ -3038,7 +3212,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="23" customFormat="1">
+    <row r="50" spans="1:16" s="23" customFormat="1" hidden="1">
       <c r="A50" s="23">
         <v>20151214</v>
       </c>
@@ -3063,14 +3237,14 @@
       <c r="I50" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="K50" s="36"/>
-      <c r="L50" s="37"/>
-      <c r="M50" s="37"/>
-      <c r="N50" s="37"/>
-      <c r="O50" s="37"/>
-      <c r="P50" s="37"/>
-    </row>
-    <row r="51" spans="1:16" ht="42">
+      <c r="K50" s="46"/>
+      <c r="L50" s="47"/>
+      <c r="M50" s="47"/>
+      <c r="N50" s="47"/>
+      <c r="O50" s="47"/>
+      <c r="P50" s="47"/>
+    </row>
+    <row r="51" spans="1:16" ht="42" hidden="1">
       <c r="A51" s="26">
         <v>20151215</v>
       </c>
@@ -3096,7 +3270,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="26" customFormat="1">
+    <row r="52" spans="1:16" s="26" customFormat="1" hidden="1">
       <c r="A52" s="26">
         <v>20151214</v>
       </c>
@@ -3121,14 +3295,14 @@
       <c r="I52" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="K52" s="36"/>
-      <c r="L52" s="37"/>
-      <c r="M52" s="37"/>
-      <c r="N52" s="37"/>
-      <c r="O52" s="37"/>
-      <c r="P52" s="37"/>
-    </row>
-    <row r="53" spans="1:16" s="27" customFormat="1">
+      <c r="K52" s="46"/>
+      <c r="L52" s="47"/>
+      <c r="M52" s="47"/>
+      <c r="N52" s="47"/>
+      <c r="O52" s="47"/>
+      <c r="P52" s="47"/>
+    </row>
+    <row r="53" spans="1:16" s="27" customFormat="1" hidden="1">
       <c r="A53" s="27">
         <v>20151218</v>
       </c>
@@ -3154,7 +3328,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" hidden="1">
       <c r="A54" s="1">
         <v>20151223</v>
       </c>
@@ -3177,7 +3351,7 @@
         <v>-4074</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" hidden="1">
       <c r="A55" s="1">
         <v>20151225</v>
       </c>
@@ -3200,7 +3374,7 @@
         <v>4116</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="42">
+    <row r="56" spans="1:16" ht="42" hidden="1">
       <c r="A56" s="1">
         <v>20151225</v>
       </c>
@@ -3226,7 +3400,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" hidden="1">
       <c r="A57" s="1">
         <v>20151229</v>
       </c>
@@ -3252,7 +3426,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" hidden="1">
       <c r="A58" s="1">
         <v>20161014</v>
       </c>
@@ -3278,7 +3452,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" hidden="1">
       <c r="A59" s="1">
         <v>20160106</v>
       </c>
@@ -3302,7 +3476,7 @@
       </c>
       <c r="I59" s="21"/>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" hidden="1">
       <c r="A60" s="1">
         <v>20160106</v>
       </c>
@@ -3328,7 +3502,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" hidden="1">
       <c r="A61" s="1">
         <v>20160111</v>
       </c>
@@ -3354,7 +3528,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" hidden="1">
       <c r="A62" s="1">
         <v>20160111</v>
       </c>
@@ -3380,7 +3554,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" hidden="1">
       <c r="A63" s="1">
         <v>20160112</v>
       </c>
@@ -3406,7 +3580,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" hidden="1">
       <c r="A64" s="1">
         <v>20160111</v>
       </c>
@@ -3429,7 +3603,7 @@
         <v>-2331</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:16">
       <c r="A65" s="1">
         <v>20160113</v>
       </c>
@@ -3455,7 +3629,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:16" hidden="1">
       <c r="A66" s="1">
         <v>20160113</v>
       </c>
@@ -3481,16 +3655,2118 @@
         <v>146</v>
       </c>
     </row>
+    <row r="67" spans="1:16">
+      <c r="A67" s="1">
+        <v>20160114</v>
+      </c>
+      <c r="B67" s="34">
+        <v>600363</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="1">
+        <v>300</v>
+      </c>
+      <c r="F67" s="1">
+        <v>12.75</v>
+      </c>
+      <c r="G67" s="1">
+        <v>-3825</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" hidden="1">
+      <c r="A68" s="1">
+        <v>20160119</v>
+      </c>
+      <c r="B68" s="26">
+        <v>600598</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="1">
+        <v>300</v>
+      </c>
+      <c r="F68" s="1">
+        <v>11.28</v>
+      </c>
+      <c r="G68" s="1">
+        <v>-3384</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" hidden="1">
+      <c r="A69" s="1">
+        <v>20160120</v>
+      </c>
+      <c r="B69" s="34">
+        <v>600598</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E69" s="1">
+        <v>300</v>
+      </c>
+      <c r="F69" s="1">
+        <v>11.46</v>
+      </c>
+      <c r="G69" s="1">
+        <v>3438</v>
+      </c>
+      <c r="I69" s="47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
+      <c r="A70" s="1">
+        <v>20160120</v>
+      </c>
+      <c r="B70" s="34">
+        <v>600363</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E70" s="1">
+        <v>300</v>
+      </c>
+      <c r="F70" s="1">
+        <v>14.49</v>
+      </c>
+      <c r="G70" s="1">
+        <v>4347</v>
+      </c>
+      <c r="I70" s="47"/>
+    </row>
+    <row r="71" spans="1:16" hidden="1">
+      <c r="A71" s="1">
+        <v>20160122</v>
+      </c>
+      <c r="B71" s="36">
+        <v>600598</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="1">
+        <v>800</v>
+      </c>
+      <c r="F71" s="1">
+        <v>11</v>
+      </c>
+      <c r="G71" s="1">
+        <v>8800</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" s="36" customFormat="1" hidden="1">
+      <c r="A72" s="36">
+        <v>20160125</v>
+      </c>
+      <c r="B72" s="36">
+        <v>600036</v>
+      </c>
+      <c r="C72" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D72" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" s="36">
+        <v>400</v>
+      </c>
+      <c r="F72" s="36">
+        <v>15.27</v>
+      </c>
+      <c r="G72" s="36">
+        <v>-6108</v>
+      </c>
+      <c r="I72" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="K72" s="46"/>
+      <c r="L72" s="47"/>
+      <c r="M72" s="47"/>
+      <c r="N72" s="47"/>
+      <c r="O72" s="47"/>
+      <c r="P72" s="47"/>
+    </row>
+    <row r="73" spans="1:16" s="38" customFormat="1" ht="63" hidden="1">
+      <c r="A73" s="38">
+        <v>20160126</v>
+      </c>
+      <c r="B73" s="38">
+        <v>2594</v>
+      </c>
+      <c r="C73" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="D73" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" s="38">
+        <v>100</v>
+      </c>
+      <c r="F73" s="38">
+        <v>53.27</v>
+      </c>
+      <c r="G73" s="38">
+        <v>-5327</v>
+      </c>
+      <c r="I73" s="37" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" hidden="1">
+      <c r="A74" s="38">
+        <v>20160127</v>
+      </c>
+      <c r="B74" s="26">
+        <v>2673</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" s="1">
+        <v>200</v>
+      </c>
+      <c r="F74" s="1">
+        <v>23.27</v>
+      </c>
+      <c r="G74" s="1">
+        <v>-4654</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" s="43" customFormat="1" hidden="1">
+      <c r="A75" s="43">
+        <v>20150831</v>
+      </c>
+      <c r="B75" s="43">
+        <v>601169</v>
+      </c>
+      <c r="C75" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D75" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E75" s="43">
+        <v>100</v>
+      </c>
+      <c r="F75" s="43">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="G75" s="43">
+        <v>862</v>
+      </c>
+      <c r="I75" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" s="43" customFormat="1" hidden="1">
+      <c r="A76" s="43">
+        <v>20160204</v>
+      </c>
+      <c r="B76" s="43">
+        <v>601169</v>
+      </c>
+      <c r="C76" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D76" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="43">
+        <v>500</v>
+      </c>
+      <c r="F76" s="43">
+        <v>9.6</v>
+      </c>
+      <c r="G76" s="43">
+        <v>-4800</v>
+      </c>
+      <c r="I76" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" s="45" customFormat="1" hidden="1">
+      <c r="A77" s="45">
+        <v>20160224</v>
+      </c>
+      <c r="B77" s="45">
+        <v>2594</v>
+      </c>
+      <c r="C77" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="D77" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="E77" s="45">
+        <v>100</v>
+      </c>
+      <c r="F77" s="45">
+        <v>54.6</v>
+      </c>
+      <c r="G77" s="45">
+        <v>5460</v>
+      </c>
+      <c r="I77" s="44" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="C1:C66"/>
-  <mergeCells count="4">
+  <autoFilter ref="C1:C77">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="联创光电"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <mergeCells count="6">
+    <mergeCell ref="K72:P72"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="K48:P48"/>
     <mergeCell ref="K50:P50"/>
     <mergeCell ref="K52:P52"/>
+    <mergeCell ref="I69:I70"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D2:F180"/>
+  <sheetViews>
+    <sheetView topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="4:6">
+      <c r="D2" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="39"/>
+    </row>
+    <row r="3" spans="4:6">
+      <c r="D3" s="51"/>
+      <c r="E3" s="40" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6">
+      <c r="D4" s="41"/>
+      <c r="E4" s="40">
+        <v>163</v>
+      </c>
+      <c r="F4" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6">
+      <c r="D5" s="41"/>
+      <c r="E5" s="40">
+        <v>170</v>
+      </c>
+      <c r="F5" s="41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6">
+      <c r="D6" s="41"/>
+      <c r="E6" s="40">
+        <v>177</v>
+      </c>
+      <c r="F6" s="41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6">
+      <c r="D7" s="41"/>
+      <c r="E7" s="40">
+        <v>2</v>
+      </c>
+      <c r="F7" s="41">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6">
+      <c r="D8" s="41"/>
+      <c r="E8" s="40">
+        <v>3</v>
+      </c>
+      <c r="F8" s="41">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6">
+      <c r="D9" s="41"/>
+      <c r="E9" s="40">
+        <v>4</v>
+      </c>
+      <c r="F9" s="41">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6">
+      <c r="D10" s="41"/>
+      <c r="E10" s="40">
+        <v>5</v>
+      </c>
+      <c r="F10" s="41">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6">
+      <c r="D11" s="41"/>
+      <c r="E11" s="40">
+        <v>6</v>
+      </c>
+      <c r="F11" s="41">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6">
+      <c r="D12" s="41"/>
+      <c r="E12" s="40">
+        <v>7</v>
+      </c>
+      <c r="F12" s="41">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6">
+      <c r="D13" s="41"/>
+      <c r="E13" s="40">
+        <v>8</v>
+      </c>
+      <c r="F13" s="41">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6">
+      <c r="D14" s="41"/>
+      <c r="E14" s="40">
+        <v>9</v>
+      </c>
+      <c r="F14" s="41">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6">
+      <c r="D15" s="41"/>
+      <c r="E15" s="40">
+        <v>10</v>
+      </c>
+      <c r="F15" s="41">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6">
+      <c r="D16" s="41"/>
+      <c r="E16" s="40">
+        <v>11</v>
+      </c>
+      <c r="F16" s="41">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6">
+      <c r="D17" s="41"/>
+      <c r="E17" s="40">
+        <v>12</v>
+      </c>
+      <c r="F17" s="41">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6">
+      <c r="D18" s="41"/>
+      <c r="E18" s="40">
+        <v>13</v>
+      </c>
+      <c r="F18" s="41">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6">
+      <c r="D19" s="41"/>
+      <c r="E19" s="40">
+        <v>14</v>
+      </c>
+      <c r="F19" s="41">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6">
+      <c r="D20" s="41"/>
+      <c r="E20" s="40">
+        <v>15</v>
+      </c>
+      <c r="F20" s="41">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6">
+      <c r="D21" s="41"/>
+      <c r="E21" s="40">
+        <v>16</v>
+      </c>
+      <c r="F21" s="41">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6">
+      <c r="D22" s="41"/>
+      <c r="E22" s="40">
+        <v>17</v>
+      </c>
+      <c r="F22" s="41">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6">
+      <c r="D23" s="41"/>
+      <c r="E23" s="40">
+        <v>18</v>
+      </c>
+      <c r="F23" s="41">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6">
+      <c r="D24" s="41"/>
+      <c r="E24" s="40">
+        <v>19</v>
+      </c>
+      <c r="F24" s="41">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6">
+      <c r="D25" s="41"/>
+      <c r="E25" s="40">
+        <v>20</v>
+      </c>
+      <c r="F25" s="41">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6">
+      <c r="D26" s="41"/>
+      <c r="E26" s="40">
+        <v>21</v>
+      </c>
+      <c r="F26" s="41">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6">
+      <c r="D27" s="41"/>
+      <c r="E27" s="40">
+        <v>22</v>
+      </c>
+      <c r="F27" s="41">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6">
+      <c r="D28" s="41"/>
+      <c r="E28" s="40">
+        <v>23</v>
+      </c>
+      <c r="F28" s="41">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6">
+      <c r="D29" s="41"/>
+      <c r="E29" s="40">
+        <v>24</v>
+      </c>
+      <c r="F29" s="41">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6">
+      <c r="D30" s="41"/>
+      <c r="E30" s="40">
+        <v>169</v>
+      </c>
+      <c r="F30" s="41">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6">
+      <c r="D31" s="41"/>
+      <c r="E31" s="40">
+        <v>25</v>
+      </c>
+      <c r="F31" s="41">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="32" spans="4:6">
+      <c r="D32" s="41"/>
+      <c r="E32" s="40">
+        <v>26</v>
+      </c>
+      <c r="F32" s="41">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6">
+      <c r="D33" s="41"/>
+      <c r="E33" s="40">
+        <v>27</v>
+      </c>
+      <c r="F33" s="41">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6">
+      <c r="D34" s="41"/>
+      <c r="E34" s="40">
+        <v>28</v>
+      </c>
+      <c r="F34" s="41">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6">
+      <c r="D35" s="41"/>
+      <c r="E35" s="40">
+        <v>29</v>
+      </c>
+      <c r="F35" s="41">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6">
+      <c r="D36" s="41"/>
+      <c r="E36" s="40">
+        <v>30</v>
+      </c>
+      <c r="F36" s="41">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6">
+      <c r="D37" s="41"/>
+      <c r="E37" s="40">
+        <v>31</v>
+      </c>
+      <c r="F37" s="41">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6">
+      <c r="D38" s="41"/>
+      <c r="E38" s="40">
+        <v>32</v>
+      </c>
+      <c r="F38" s="41">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6">
+      <c r="D39" s="41"/>
+      <c r="E39" s="40">
+        <v>33</v>
+      </c>
+      <c r="F39" s="41">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6">
+      <c r="D40" s="41"/>
+      <c r="E40" s="40">
+        <v>34</v>
+      </c>
+      <c r="F40" s="41">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6">
+      <c r="D41" s="41"/>
+      <c r="E41" s="40">
+        <v>35</v>
+      </c>
+      <c r="F41" s="41">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6">
+      <c r="D42" s="41"/>
+      <c r="E42" s="40">
+        <v>36</v>
+      </c>
+      <c r="F42" s="41">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6">
+      <c r="D43" s="41"/>
+      <c r="E43" s="40">
+        <v>37</v>
+      </c>
+      <c r="F43" s="41">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6">
+      <c r="D44" s="41"/>
+      <c r="E44" s="40">
+        <v>38</v>
+      </c>
+      <c r="F44" s="41">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="45" spans="4:6">
+      <c r="D45" s="41"/>
+      <c r="E45" s="40">
+        <v>39</v>
+      </c>
+      <c r="F45" s="41">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6">
+      <c r="D46" s="41"/>
+      <c r="E46" s="40">
+        <v>40</v>
+      </c>
+      <c r="F46" s="41">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6">
+      <c r="D47" s="41"/>
+      <c r="E47" s="40">
+        <v>41</v>
+      </c>
+      <c r="F47" s="41">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6">
+      <c r="D48" s="41"/>
+      <c r="E48" s="40">
+        <v>42</v>
+      </c>
+      <c r="F48" s="41">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6">
+      <c r="D49" s="41"/>
+      <c r="E49" s="40">
+        <v>176</v>
+      </c>
+      <c r="F49" s="41">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="50" spans="4:6">
+      <c r="D50" s="41"/>
+      <c r="E50" s="40">
+        <v>43</v>
+      </c>
+      <c r="F50" s="41">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="51" spans="4:6">
+      <c r="D51" s="41"/>
+      <c r="E51" s="40">
+        <v>44</v>
+      </c>
+      <c r="F51" s="41">
+        <v>3010</v>
+      </c>
+    </row>
+    <row r="52" spans="4:6">
+      <c r="D52" s="41"/>
+      <c r="E52" s="40">
+        <v>45</v>
+      </c>
+      <c r="F52" s="41">
+        <v>3063</v>
+      </c>
+    </row>
+    <row r="53" spans="4:6">
+      <c r="D53" s="41"/>
+      <c r="E53" s="40">
+        <v>46</v>
+      </c>
+      <c r="F53" s="41">
+        <v>3912</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6">
+      <c r="D54" s="41"/>
+      <c r="E54" s="40">
+        <v>47</v>
+      </c>
+      <c r="F54" s="41">
+        <v>3914</v>
+      </c>
+    </row>
+    <row r="55" spans="4:6">
+      <c r="D55" s="41"/>
+      <c r="E55" s="40">
+        <v>48</v>
+      </c>
+      <c r="F55" s="41">
+        <v>3917</v>
+      </c>
+    </row>
+    <row r="56" spans="4:6">
+      <c r="D56" s="41"/>
+      <c r="E56" s="40">
+        <v>49</v>
+      </c>
+      <c r="F56" s="41">
+        <v>3972</v>
+      </c>
+    </row>
+    <row r="57" spans="4:6">
+      <c r="D57" s="41"/>
+      <c r="E57" s="40">
+        <v>50</v>
+      </c>
+      <c r="F57" s="41">
+        <v>3990</v>
+      </c>
+    </row>
+    <row r="58" spans="4:6">
+      <c r="D58" s="41"/>
+      <c r="E58" s="40">
+        <v>51</v>
+      </c>
+      <c r="F58" s="41">
+        <v>4163</v>
+      </c>
+    </row>
+    <row r="59" spans="4:6">
+      <c r="D59" s="41"/>
+      <c r="E59" s="40">
+        <v>52</v>
+      </c>
+      <c r="F59" s="41">
+        <v>4363</v>
+      </c>
+    </row>
+    <row r="60" spans="4:6">
+      <c r="D60" s="41"/>
+      <c r="E60" s="40">
+        <v>53</v>
+      </c>
+      <c r="F60" s="41">
+        <v>4534</v>
+      </c>
+    </row>
+    <row r="61" spans="4:6">
+      <c r="D61" s="41"/>
+      <c r="E61" s="40">
+        <v>54</v>
+      </c>
+      <c r="F61" s="41">
+        <v>5458</v>
+      </c>
+    </row>
+    <row r="62" spans="4:6">
+      <c r="D62" s="41"/>
+      <c r="E62" s="40">
+        <v>55</v>
+      </c>
+      <c r="F62" s="41">
+        <v>5955</v>
+      </c>
+    </row>
+    <row r="63" spans="4:6">
+      <c r="D63" s="41"/>
+      <c r="E63" s="40">
+        <v>173</v>
+      </c>
+      <c r="F63" s="41">
+        <v>6578</v>
+      </c>
+    </row>
+    <row r="64" spans="4:6">
+      <c r="D64" s="41"/>
+      <c r="E64" s="40">
+        <v>56</v>
+      </c>
+      <c r="F64" s="41">
+        <v>7212</v>
+      </c>
+    </row>
+    <row r="65" spans="4:6">
+      <c r="D65" s="41"/>
+      <c r="E65" s="40">
+        <v>57</v>
+      </c>
+      <c r="F65" s="41">
+        <v>7680</v>
+      </c>
+    </row>
+    <row r="66" spans="4:6">
+      <c r="D66" s="41"/>
+      <c r="E66" s="40">
+        <v>58</v>
+      </c>
+      <c r="F66" s="41">
+        <v>8037</v>
+      </c>
+    </row>
+    <row r="67" spans="4:6">
+      <c r="D67" s="41"/>
+      <c r="E67" s="40">
+        <v>59</v>
+      </c>
+      <c r="F67" s="41">
+        <v>8060</v>
+      </c>
+    </row>
+    <row r="68" spans="4:6">
+      <c r="D68" s="41"/>
+      <c r="E68" s="40">
+        <v>60</v>
+      </c>
+      <c r="F68" s="41">
+        <v>8843</v>
+      </c>
+    </row>
+    <row r="69" spans="4:6">
+      <c r="D69" s="41"/>
+      <c r="E69" s="40">
+        <v>165</v>
+      </c>
+      <c r="F69" s="41">
+        <v>8865</v>
+      </c>
+    </row>
+    <row r="70" spans="4:6">
+      <c r="D70" s="41"/>
+      <c r="E70" s="40">
+        <v>61</v>
+      </c>
+      <c r="F70" s="41">
+        <v>8893</v>
+      </c>
+    </row>
+    <row r="71" spans="4:6">
+      <c r="D71" s="41"/>
+      <c r="E71" s="40">
+        <v>62</v>
+      </c>
+      <c r="F71" s="41">
+        <v>8902</v>
+      </c>
+    </row>
+    <row r="72" spans="4:6">
+      <c r="D72" s="41"/>
+      <c r="E72" s="40">
+        <v>63</v>
+      </c>
+      <c r="F72" s="41">
+        <v>9009</v>
+      </c>
+    </row>
+    <row r="73" spans="4:6">
+      <c r="D73" s="41"/>
+      <c r="E73" s="40">
+        <v>64</v>
+      </c>
+      <c r="F73" s="41">
+        <v>9084</v>
+      </c>
+    </row>
+    <row r="74" spans="4:6">
+      <c r="D74" s="41"/>
+      <c r="E74" s="40">
+        <v>65</v>
+      </c>
+      <c r="F74" s="41">
+        <v>9086</v>
+      </c>
+    </row>
+    <row r="75" spans="4:6">
+      <c r="D75" s="41"/>
+      <c r="E75" s="40">
+        <v>167</v>
+      </c>
+      <c r="F75" s="41">
+        <v>9138</v>
+      </c>
+    </row>
+    <row r="76" spans="4:6">
+      <c r="D76" s="41"/>
+      <c r="E76" s="40">
+        <v>166</v>
+      </c>
+      <c r="F76" s="41">
+        <v>9859</v>
+      </c>
+    </row>
+    <row r="77" spans="4:6">
+      <c r="D77" s="41"/>
+      <c r="E77" s="40">
+        <v>66</v>
+      </c>
+      <c r="F77" s="41">
+        <v>11843</v>
+      </c>
+    </row>
+    <row r="78" spans="4:6">
+      <c r="D78" s="41"/>
+      <c r="E78" s="40">
+        <v>164</v>
+      </c>
+      <c r="F78" s="41">
+        <v>12795</v>
+      </c>
+    </row>
+    <row r="79" spans="4:6">
+      <c r="D79" s="41"/>
+      <c r="E79" s="40">
+        <v>175</v>
+      </c>
+      <c r="F79" s="41">
+        <v>12823</v>
+      </c>
+    </row>
+    <row r="80" spans="4:6">
+      <c r="D80" s="41"/>
+      <c r="E80" s="40">
+        <v>67</v>
+      </c>
+      <c r="F80" s="41">
+        <v>14124</v>
+      </c>
+    </row>
+    <row r="81" spans="4:6">
+      <c r="D81" s="41"/>
+      <c r="E81" s="40">
+        <v>162</v>
+      </c>
+      <c r="F81" s="41">
+        <v>14467</v>
+      </c>
+    </row>
+    <row r="82" spans="4:6">
+      <c r="D82" s="41"/>
+      <c r="E82" s="40">
+        <v>68</v>
+      </c>
+      <c r="F82" s="41">
+        <v>14629</v>
+      </c>
+    </row>
+    <row r="83" spans="4:6">
+      <c r="D83" s="41"/>
+      <c r="E83" s="40">
+        <v>69</v>
+      </c>
+      <c r="F83" s="41">
+        <v>14772</v>
+      </c>
+    </row>
+    <row r="84" spans="4:6">
+      <c r="D84" s="41"/>
+      <c r="E84" s="40">
+        <v>174</v>
+      </c>
+      <c r="F84" s="41">
+        <v>15163</v>
+      </c>
+    </row>
+    <row r="85" spans="4:6">
+      <c r="D85" s="41"/>
+      <c r="E85" s="40">
+        <v>1</v>
+      </c>
+      <c r="F85" s="41">
+        <v>16163</v>
+      </c>
+    </row>
+    <row r="86" spans="4:6">
+      <c r="D86" s="41"/>
+      <c r="E86" s="40">
+        <v>70</v>
+      </c>
+      <c r="F86" s="41">
+        <v>19692</v>
+      </c>
+    </row>
+    <row r="87" spans="4:6">
+      <c r="D87" s="41"/>
+      <c r="E87" s="40">
+        <v>71</v>
+      </c>
+      <c r="F87" s="41">
+        <v>21694</v>
+      </c>
+    </row>
+    <row r="88" spans="4:6">
+      <c r="D88" s="41"/>
+      <c r="E88" s="40">
+        <v>72</v>
+      </c>
+      <c r="F88" s="41">
+        <v>23638</v>
+      </c>
+    </row>
+    <row r="89" spans="4:6">
+      <c r="D89" s="41"/>
+      <c r="E89" s="40">
+        <v>73</v>
+      </c>
+      <c r="F89" s="41">
+        <v>24686</v>
+      </c>
+    </row>
+    <row r="90" spans="4:6">
+      <c r="D90" s="41"/>
+      <c r="E90" s="40">
+        <v>74</v>
+      </c>
+      <c r="F90" s="41">
+        <v>28286</v>
+      </c>
+    </row>
+    <row r="91" spans="4:6">
+      <c r="D91" s="41"/>
+      <c r="E91" s="40">
+        <v>75</v>
+      </c>
+      <c r="F91" s="41">
+        <v>29411</v>
+      </c>
+    </row>
+    <row r="92" spans="4:6">
+      <c r="D92" s="41"/>
+      <c r="E92" s="40">
+        <v>76</v>
+      </c>
+      <c r="F92" s="41">
+        <v>29554</v>
+      </c>
+    </row>
+    <row r="93" spans="4:6">
+      <c r="D93" s="41"/>
+      <c r="E93" s="40">
+        <v>77</v>
+      </c>
+      <c r="F93" s="41">
+        <v>29800</v>
+      </c>
+    </row>
+    <row r="94" spans="4:6">
+      <c r="D94" s="41"/>
+      <c r="E94" s="40">
+        <v>78</v>
+      </c>
+      <c r="F94" s="41">
+        <v>29801</v>
+      </c>
+    </row>
+    <row r="95" spans="4:6">
+      <c r="D95" s="41"/>
+      <c r="E95" s="40">
+        <v>79</v>
+      </c>
+      <c r="F95" s="41">
+        <v>30060</v>
+      </c>
+    </row>
+    <row r="96" spans="4:6">
+      <c r="D96" s="41"/>
+      <c r="E96" s="40">
+        <v>80</v>
+      </c>
+      <c r="F96" s="41">
+        <v>30085</v>
+      </c>
+    </row>
+    <row r="97" spans="4:6">
+      <c r="D97" s="41"/>
+      <c r="E97" s="40">
+        <v>81</v>
+      </c>
+      <c r="F97" s="41">
+        <v>30119</v>
+      </c>
+    </row>
+    <row r="98" spans="4:6">
+      <c r="D98" s="41"/>
+      <c r="E98" s="40">
+        <v>82</v>
+      </c>
+      <c r="F98" s="41">
+        <v>33743</v>
+      </c>
+    </row>
+    <row r="99" spans="4:6">
+      <c r="D99" s="41"/>
+      <c r="E99" s="40">
+        <v>83</v>
+      </c>
+      <c r="F99" s="41">
+        <v>34479</v>
+      </c>
+    </row>
+    <row r="100" spans="4:6">
+      <c r="D100" s="41"/>
+      <c r="E100" s="40">
+        <v>84</v>
+      </c>
+      <c r="F100" s="41">
+        <v>34481</v>
+      </c>
+    </row>
+    <row r="101" spans="4:6">
+      <c r="D101" s="41"/>
+      <c r="E101" s="40">
+        <v>85</v>
+      </c>
+      <c r="F101" s="41">
+        <v>34483</v>
+      </c>
+    </row>
+    <row r="102" spans="4:6">
+      <c r="D102" s="41"/>
+      <c r="E102" s="40">
+        <v>86</v>
+      </c>
+      <c r="F102" s="41">
+        <v>34484</v>
+      </c>
+    </row>
+    <row r="103" spans="4:6">
+      <c r="D103" s="41"/>
+      <c r="E103" s="40">
+        <v>87</v>
+      </c>
+      <c r="F103" s="41">
+        <v>34488</v>
+      </c>
+    </row>
+    <row r="104" spans="4:6">
+      <c r="D104" s="41"/>
+      <c r="E104" s="40">
+        <v>88</v>
+      </c>
+      <c r="F104" s="41">
+        <v>34492</v>
+      </c>
+    </row>
+    <row r="105" spans="4:6">
+      <c r="D105" s="41"/>
+      <c r="E105" s="40">
+        <v>89</v>
+      </c>
+      <c r="F105" s="41">
+        <v>34493</v>
+      </c>
+    </row>
+    <row r="106" spans="4:6">
+      <c r="D106" s="41"/>
+      <c r="E106" s="40">
+        <v>90</v>
+      </c>
+      <c r="F106" s="41">
+        <v>34494</v>
+      </c>
+    </row>
+    <row r="107" spans="4:6">
+      <c r="D107" s="41"/>
+      <c r="E107" s="40">
+        <v>91</v>
+      </c>
+      <c r="F107" s="41">
+        <v>34495</v>
+      </c>
+    </row>
+    <row r="108" spans="4:6">
+      <c r="D108" s="41"/>
+      <c r="E108" s="40">
+        <v>92</v>
+      </c>
+      <c r="F108" s="41">
+        <v>34496</v>
+      </c>
+    </row>
+    <row r="109" spans="4:6">
+      <c r="D109" s="41"/>
+      <c r="E109" s="40">
+        <v>93</v>
+      </c>
+      <c r="F109" s="41">
+        <v>34498</v>
+      </c>
+    </row>
+    <row r="110" spans="4:6">
+      <c r="D110" s="41"/>
+      <c r="E110" s="40">
+        <v>94</v>
+      </c>
+      <c r="F110" s="41">
+        <v>35253</v>
+      </c>
+    </row>
+    <row r="111" spans="4:6">
+      <c r="D111" s="41"/>
+      <c r="E111" s="40">
+        <v>95</v>
+      </c>
+      <c r="F111" s="41">
+        <v>35255</v>
+      </c>
+    </row>
+    <row r="112" spans="4:6">
+      <c r="D112" s="41"/>
+      <c r="E112" s="40">
+        <v>96</v>
+      </c>
+      <c r="F112" s="41">
+        <v>36070</v>
+      </c>
+    </row>
+    <row r="113" spans="4:6">
+      <c r="D113" s="41"/>
+      <c r="E113" s="40">
+        <v>97</v>
+      </c>
+      <c r="F113" s="41">
+        <v>36071</v>
+      </c>
+    </row>
+    <row r="114" spans="4:6">
+      <c r="D114" s="41"/>
+      <c r="E114" s="40">
+        <v>98</v>
+      </c>
+      <c r="F114" s="41">
+        <v>36075</v>
+      </c>
+    </row>
+    <row r="115" spans="4:6">
+      <c r="D115" s="41"/>
+      <c r="E115" s="40">
+        <v>99</v>
+      </c>
+      <c r="F115" s="41">
+        <v>36080</v>
+      </c>
+    </row>
+    <row r="116" spans="4:6">
+      <c r="D116" s="41"/>
+      <c r="E116" s="40">
+        <v>100</v>
+      </c>
+      <c r="F116" s="41">
+        <v>36082</v>
+      </c>
+    </row>
+    <row r="117" spans="4:6">
+      <c r="D117" s="41"/>
+      <c r="E117" s="40">
+        <v>101</v>
+      </c>
+      <c r="F117" s="41">
+        <v>36086</v>
+      </c>
+    </row>
+    <row r="118" spans="4:6">
+      <c r="D118" s="41"/>
+      <c r="E118" s="40">
+        <v>102</v>
+      </c>
+      <c r="F118" s="41">
+        <v>36087</v>
+      </c>
+    </row>
+    <row r="119" spans="4:6">
+      <c r="D119" s="41"/>
+      <c r="E119" s="40">
+        <v>103</v>
+      </c>
+      <c r="F119" s="41">
+        <v>36089</v>
+      </c>
+    </row>
+    <row r="120" spans="4:6">
+      <c r="D120" s="41"/>
+      <c r="E120" s="40">
+        <v>104</v>
+      </c>
+      <c r="F120" s="41">
+        <v>36091</v>
+      </c>
+    </row>
+    <row r="121" spans="4:6">
+      <c r="D121" s="41"/>
+      <c r="E121" s="40">
+        <v>105</v>
+      </c>
+      <c r="F121" s="41">
+        <v>36092</v>
+      </c>
+    </row>
+    <row r="122" spans="4:6">
+      <c r="D122" s="41"/>
+      <c r="E122" s="40">
+        <v>106</v>
+      </c>
+      <c r="F122" s="41">
+        <v>36093</v>
+      </c>
+    </row>
+    <row r="123" spans="4:6">
+      <c r="D123" s="41"/>
+      <c r="E123" s="40">
+        <v>107</v>
+      </c>
+      <c r="F123" s="41">
+        <v>36094</v>
+      </c>
+    </row>
+    <row r="124" spans="4:6">
+      <c r="D124" s="41"/>
+      <c r="E124" s="40">
+        <v>108</v>
+      </c>
+      <c r="F124" s="41">
+        <v>36099</v>
+      </c>
+    </row>
+    <row r="125" spans="4:6">
+      <c r="D125" s="41"/>
+      <c r="E125" s="40">
+        <v>109</v>
+      </c>
+      <c r="F125" s="41">
+        <v>36102</v>
+      </c>
+    </row>
+    <row r="126" spans="4:6">
+      <c r="D126" s="41"/>
+      <c r="E126" s="40">
+        <v>110</v>
+      </c>
+      <c r="F126" s="41">
+        <v>36103</v>
+      </c>
+    </row>
+    <row r="127" spans="4:6">
+      <c r="D127" s="41"/>
+      <c r="E127" s="40">
+        <v>111</v>
+      </c>
+      <c r="F127" s="41">
+        <v>36104</v>
+      </c>
+    </row>
+    <row r="128" spans="4:6">
+      <c r="D128" s="41"/>
+      <c r="E128" s="40">
+        <v>112</v>
+      </c>
+      <c r="F128" s="41">
+        <v>36106</v>
+      </c>
+    </row>
+    <row r="129" spans="4:6">
+      <c r="D129" s="41"/>
+      <c r="E129" s="40">
+        <v>113</v>
+      </c>
+      <c r="F129" s="41">
+        <v>36108</v>
+      </c>
+    </row>
+    <row r="130" spans="4:6">
+      <c r="D130" s="41"/>
+      <c r="E130" s="40">
+        <v>114</v>
+      </c>
+      <c r="F130" s="41">
+        <v>36111</v>
+      </c>
+    </row>
+    <row r="131" spans="4:6">
+      <c r="D131" s="41"/>
+      <c r="E131" s="40">
+        <v>115</v>
+      </c>
+      <c r="F131" s="41">
+        <v>36112</v>
+      </c>
+    </row>
+    <row r="132" spans="4:6">
+      <c r="D132" s="41"/>
+      <c r="E132" s="40">
+        <v>116</v>
+      </c>
+      <c r="F132" s="41">
+        <v>36113</v>
+      </c>
+    </row>
+    <row r="133" spans="4:6">
+      <c r="D133" s="41"/>
+      <c r="E133" s="40">
+        <v>117</v>
+      </c>
+      <c r="F133" s="41">
+        <v>36117</v>
+      </c>
+    </row>
+    <row r="134" spans="4:6">
+      <c r="D134" s="41"/>
+      <c r="E134" s="40">
+        <v>118</v>
+      </c>
+      <c r="F134" s="41">
+        <v>36122</v>
+      </c>
+    </row>
+    <row r="135" spans="4:6">
+      <c r="D135" s="41"/>
+      <c r="E135" s="40">
+        <v>119</v>
+      </c>
+      <c r="F135" s="41">
+        <v>36126</v>
+      </c>
+    </row>
+    <row r="136" spans="4:6">
+      <c r="D136" s="41"/>
+      <c r="E136" s="40">
+        <v>120</v>
+      </c>
+      <c r="F136" s="41">
+        <v>36127</v>
+      </c>
+    </row>
+    <row r="137" spans="4:6">
+      <c r="D137" s="41"/>
+      <c r="E137" s="40">
+        <v>121</v>
+      </c>
+      <c r="F137" s="41">
+        <v>36129</v>
+      </c>
+    </row>
+    <row r="138" spans="4:6">
+      <c r="D138" s="41"/>
+      <c r="E138" s="40">
+        <v>122</v>
+      </c>
+      <c r="F138" s="41">
+        <v>36132</v>
+      </c>
+    </row>
+    <row r="139" spans="4:6">
+      <c r="D139" s="41"/>
+      <c r="E139" s="40">
+        <v>123</v>
+      </c>
+      <c r="F139" s="41">
+        <v>36140</v>
+      </c>
+    </row>
+    <row r="140" spans="4:6">
+      <c r="D140" s="41"/>
+      <c r="E140" s="40">
+        <v>124</v>
+      </c>
+      <c r="F140" s="41">
+        <v>36144</v>
+      </c>
+    </row>
+    <row r="141" spans="4:6">
+      <c r="D141" s="41"/>
+      <c r="E141" s="40">
+        <v>125</v>
+      </c>
+      <c r="F141" s="41">
+        <v>36148</v>
+      </c>
+    </row>
+    <row r="142" spans="4:6">
+      <c r="D142" s="41"/>
+      <c r="E142" s="40">
+        <v>126</v>
+      </c>
+      <c r="F142" s="41">
+        <v>36149</v>
+      </c>
+    </row>
+    <row r="143" spans="4:6">
+      <c r="D143" s="41"/>
+      <c r="E143" s="40">
+        <v>127</v>
+      </c>
+      <c r="F143" s="41">
+        <v>36150</v>
+      </c>
+    </row>
+    <row r="144" spans="4:6">
+      <c r="D144" s="41"/>
+      <c r="E144" s="40">
+        <v>128</v>
+      </c>
+      <c r="F144" s="41">
+        <v>36153</v>
+      </c>
+    </row>
+    <row r="145" spans="4:6">
+      <c r="D145" s="41"/>
+      <c r="E145" s="40">
+        <v>129</v>
+      </c>
+      <c r="F145" s="41">
+        <v>36155</v>
+      </c>
+    </row>
+    <row r="146" spans="4:6">
+      <c r="D146" s="41"/>
+      <c r="E146" s="40">
+        <v>130</v>
+      </c>
+      <c r="F146" s="41">
+        <v>36156</v>
+      </c>
+    </row>
+    <row r="147" spans="4:6">
+      <c r="D147" s="41"/>
+      <c r="E147" s="40">
+        <v>131</v>
+      </c>
+      <c r="F147" s="41">
+        <v>36159</v>
+      </c>
+    </row>
+    <row r="148" spans="4:6">
+      <c r="D148" s="41"/>
+      <c r="E148" s="40">
+        <v>132</v>
+      </c>
+      <c r="F148" s="41">
+        <v>36163</v>
+      </c>
+    </row>
+    <row r="149" spans="4:6">
+      <c r="D149" s="41"/>
+      <c r="E149" s="40">
+        <v>133</v>
+      </c>
+      <c r="F149" s="41">
+        <v>36164</v>
+      </c>
+    </row>
+    <row r="150" spans="4:6">
+      <c r="D150" s="41"/>
+      <c r="E150" s="40">
+        <v>134</v>
+      </c>
+      <c r="F150" s="41">
+        <v>36176</v>
+      </c>
+    </row>
+    <row r="151" spans="4:6">
+      <c r="D151" s="41"/>
+      <c r="E151" s="40">
+        <v>135</v>
+      </c>
+      <c r="F151" s="41">
+        <v>36237</v>
+      </c>
+    </row>
+    <row r="152" spans="4:6">
+      <c r="D152" s="41"/>
+      <c r="E152" s="40">
+        <v>136</v>
+      </c>
+      <c r="F152" s="41">
+        <v>36306</v>
+      </c>
+    </row>
+    <row r="153" spans="4:6">
+      <c r="D153" s="41"/>
+      <c r="E153" s="40">
+        <v>137</v>
+      </c>
+      <c r="F153" s="41">
+        <v>36314</v>
+      </c>
+    </row>
+    <row r="154" spans="4:6">
+      <c r="D154" s="41"/>
+      <c r="E154" s="40">
+        <v>138</v>
+      </c>
+      <c r="F154" s="41">
+        <v>36317</v>
+      </c>
+    </row>
+    <row r="155" spans="4:6">
+      <c r="D155" s="41"/>
+      <c r="E155" s="40">
+        <v>139</v>
+      </c>
+      <c r="F155" s="41">
+        <v>36647</v>
+      </c>
+    </row>
+    <row r="156" spans="4:6">
+      <c r="D156" s="41"/>
+      <c r="E156" s="40">
+        <v>140</v>
+      </c>
+      <c r="F156" s="41">
+        <v>36702</v>
+      </c>
+    </row>
+    <row r="157" spans="4:6">
+      <c r="D157" s="41"/>
+      <c r="E157" s="40">
+        <v>141</v>
+      </c>
+      <c r="F157" s="41">
+        <v>36876</v>
+      </c>
+    </row>
+    <row r="158" spans="4:6">
+      <c r="D158" s="41"/>
+      <c r="E158" s="40">
+        <v>142</v>
+      </c>
+      <c r="F158" s="41">
+        <v>39805</v>
+      </c>
+    </row>
+    <row r="159" spans="4:6">
+      <c r="D159" s="41"/>
+      <c r="E159" s="40">
+        <v>143</v>
+      </c>
+      <c r="F159" s="41">
+        <v>40024</v>
+      </c>
+    </row>
+    <row r="160" spans="4:6">
+      <c r="D160" s="41"/>
+      <c r="E160" s="40">
+        <v>144</v>
+      </c>
+      <c r="F160" s="41">
+        <v>44341</v>
+      </c>
+    </row>
+    <row r="161" spans="4:6">
+      <c r="D161" s="41"/>
+      <c r="E161" s="40">
+        <v>145</v>
+      </c>
+      <c r="F161" s="41">
+        <v>46481</v>
+      </c>
+    </row>
+    <row r="162" spans="4:6">
+      <c r="D162" s="41"/>
+      <c r="E162" s="40">
+        <v>146</v>
+      </c>
+      <c r="F162" s="41">
+        <v>47151</v>
+      </c>
+    </row>
+    <row r="163" spans="4:6">
+      <c r="D163" s="41"/>
+      <c r="E163" s="40">
+        <v>147</v>
+      </c>
+      <c r="F163" s="41">
+        <v>51614</v>
+      </c>
+    </row>
+    <row r="164" spans="4:6">
+      <c r="D164" s="41"/>
+      <c r="E164" s="40">
+        <v>148</v>
+      </c>
+      <c r="F164" s="41">
+        <v>51628</v>
+      </c>
+    </row>
+    <row r="165" spans="4:6">
+      <c r="D165" s="41"/>
+      <c r="E165" s="40">
+        <v>149</v>
+      </c>
+      <c r="F165" s="41">
+        <v>51629</v>
+      </c>
+    </row>
+    <row r="166" spans="4:6">
+      <c r="D166" s="41"/>
+      <c r="E166" s="40">
+        <v>150</v>
+      </c>
+      <c r="F166" s="41">
+        <v>51767</v>
+      </c>
+    </row>
+    <row r="167" spans="4:6">
+      <c r="D167" s="41"/>
+      <c r="E167" s="40">
+        <v>151</v>
+      </c>
+      <c r="F167" s="41">
+        <v>51846</v>
+      </c>
+    </row>
+    <row r="168" spans="4:6">
+      <c r="D168" s="41"/>
+      <c r="E168" s="40">
+        <v>152</v>
+      </c>
+      <c r="F168" s="41">
+        <v>51872</v>
+      </c>
+    </row>
+    <row r="169" spans="4:6">
+      <c r="D169" s="41"/>
+      <c r="E169" s="40">
+        <v>153</v>
+      </c>
+      <c r="F169" s="41">
+        <v>51882</v>
+      </c>
+    </row>
+    <row r="170" spans="4:6">
+      <c r="D170" s="41"/>
+      <c r="E170" s="40">
+        <v>154</v>
+      </c>
+      <c r="F170" s="41">
+        <v>52157</v>
+      </c>
+    </row>
+    <row r="171" spans="4:6">
+      <c r="D171" s="41"/>
+      <c r="E171" s="40">
+        <v>155</v>
+      </c>
+      <c r="F171" s="41">
+        <v>52245</v>
+      </c>
+    </row>
+    <row r="172" spans="4:6">
+      <c r="D172" s="41"/>
+      <c r="E172" s="40">
+        <v>156</v>
+      </c>
+      <c r="F172" s="41">
+        <v>52295</v>
+      </c>
+    </row>
+    <row r="173" spans="4:6">
+      <c r="D173" s="41"/>
+      <c r="E173" s="40">
+        <v>157</v>
+      </c>
+      <c r="F173" s="41">
+        <v>52304</v>
+      </c>
+    </row>
+    <row r="174" spans="4:6">
+      <c r="D174" s="41"/>
+      <c r="E174" s="40">
+        <v>158</v>
+      </c>
+      <c r="F174" s="41">
+        <v>52701</v>
+      </c>
+    </row>
+    <row r="175" spans="4:6">
+      <c r="D175" s="41"/>
+      <c r="E175" s="40">
+        <v>159</v>
+      </c>
+      <c r="F175" s="41">
+        <v>53037</v>
+      </c>
+    </row>
+    <row r="176" spans="4:6">
+      <c r="D176" s="41"/>
+      <c r="E176" s="40">
+        <v>160</v>
+      </c>
+      <c r="F176" s="41">
+        <v>54621</v>
+      </c>
+    </row>
+    <row r="177" spans="4:6">
+      <c r="D177" s="41"/>
+      <c r="E177" s="40">
+        <v>161</v>
+      </c>
+      <c r="F177" s="41">
+        <v>54709</v>
+      </c>
+    </row>
+    <row r="178" spans="4:6">
+      <c r="D178" s="41"/>
+      <c r="E178" s="40">
+        <v>168</v>
+      </c>
+      <c r="F178" s="41">
+        <v>55108</v>
+      </c>
+    </row>
+    <row r="179" spans="4:6">
+      <c r="D179" s="41"/>
+      <c r="E179" s="40">
+        <v>171</v>
+      </c>
+      <c r="F179" s="41">
+        <v>55116</v>
+      </c>
+    </row>
+    <row r="180" spans="4:6">
+      <c r="D180" s="42" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:D3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/163/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E5" r:id="rId4" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/170/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E6" r:id="rId5" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/177/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E7" r:id="rId6" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/2/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E8" r:id="rId7" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/3/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E9" r:id="rId8" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/4/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E10" r:id="rId9" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/5/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E11" r:id="rId10" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/6/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E12" r:id="rId11" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/7/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E13" r:id="rId12" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/8/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E14" r:id="rId13" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/9/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E15" r:id="rId14" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/10/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E16" r:id="rId15" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/11/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E17" r:id="rId16" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/12/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E18" r:id="rId17" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/13/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E19" r:id="rId18" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/14/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E20" r:id="rId19" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/15/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E21" r:id="rId20" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/16/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E22" r:id="rId21" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/17/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E23" r:id="rId22" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/18/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E24" r:id="rId23" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/19/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E25" r:id="rId24" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/20/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E26" r:id="rId25" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/21/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E27" r:id="rId26" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/22/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E28" r:id="rId27" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/23/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E29" r:id="rId28" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/24/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E30" r:id="rId29" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/169/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E31" r:id="rId30" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/25/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E32" r:id="rId31" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/26/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E33" r:id="rId32" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/27/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E34" r:id="rId33" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/28/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E35" r:id="rId34" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/29/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E36" r:id="rId35" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/30/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E37" r:id="rId36" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/31/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E38" r:id="rId37" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/32/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E39" r:id="rId38" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/33/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E40" r:id="rId39" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/34/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E41" r:id="rId40" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/35/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E42" r:id="rId41" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/36/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E43" r:id="rId42" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/37/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E44" r:id="rId43" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/38/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E45" r:id="rId44" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/39/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E46" r:id="rId45" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/40/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E47" r:id="rId46" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/41/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E48" r:id="rId47" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/42/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E49" r:id="rId48" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/176/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E50" r:id="rId49" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/43/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E51" r:id="rId50" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/44/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E52" r:id="rId51" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/45/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E53" r:id="rId52" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/46/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E54" r:id="rId53" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/47/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E55" r:id="rId54" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/48/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E56" r:id="rId55" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/49/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E57" r:id="rId56" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/50/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E58" r:id="rId57" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/51/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E59" r:id="rId58" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/52/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E60" r:id="rId59" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/53/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E61" r:id="rId60" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/54/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E62" r:id="rId61" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/55/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E63" r:id="rId62" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/173/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E64" r:id="rId63" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/56/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E65" r:id="rId64" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/57/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E66" r:id="rId65" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/58/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E67" r:id="rId66" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/59/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E68" r:id="rId67" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/60/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E69" r:id="rId68" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/165/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E70" r:id="rId69" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/61/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E71" r:id="rId70" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/62/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E72" r:id="rId71" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/63/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E73" r:id="rId72" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/64/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E74" r:id="rId73" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/65/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E75" r:id="rId74" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/167/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E76" r:id="rId75" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/166/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E77" r:id="rId76" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/66/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E78" r:id="rId77" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/164/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E79" r:id="rId78" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/175/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E80" r:id="rId79" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/67/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E81" r:id="rId80" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/162/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E82" r:id="rId81" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/68/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E83" r:id="rId82" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/69/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E84" r:id="rId83" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/174/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E85" r:id="rId84" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/1/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E86" r:id="rId85" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/70/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E87" r:id="rId86" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/71/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E88" r:id="rId87" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/72/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E89" r:id="rId88" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/73/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E90" r:id="rId89" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/74/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E91" r:id="rId90" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/75/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E92" r:id="rId91" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/76/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E93" r:id="rId92" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/77/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E94" r:id="rId93" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/78/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E95" r:id="rId94" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/79/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E96" r:id="rId95" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/80/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E97" r:id="rId96" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/81/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E98" r:id="rId97" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/82/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E99" r:id="rId98" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/83/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E100" r:id="rId99" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/84/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E101" r:id="rId100" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/85/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E102" r:id="rId101" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/86/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E103" r:id="rId102" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/87/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E104" r:id="rId103" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/88/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E105" r:id="rId104" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/89/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E106" r:id="rId105" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/90/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E107" r:id="rId106" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/91/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E108" r:id="rId107" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/92/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E109" r:id="rId108" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/93/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E110" r:id="rId109" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/94/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E111" r:id="rId110" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/95/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E112" r:id="rId111" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/96/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E113" r:id="rId112" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/97/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E114" r:id="rId113" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/98/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E115" r:id="rId114" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/99/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E116" r:id="rId115" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/100/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E117" r:id="rId116" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/101/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E118" r:id="rId117" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/102/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E119" r:id="rId118" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/103/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E120" r:id="rId119" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/104/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E121" r:id="rId120" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/105/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E122" r:id="rId121" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/106/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E123" r:id="rId122" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/107/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E124" r:id="rId123" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/108/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E125" r:id="rId124" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/109/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E126" r:id="rId125" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/110/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E127" r:id="rId126" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/111/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E128" r:id="rId127" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/112/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E129" r:id="rId128" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/113/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E130" r:id="rId129" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/114/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E131" r:id="rId130" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/115/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E132" r:id="rId131" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/116/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E133" r:id="rId132" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/117/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E134" r:id="rId133" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/118/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E135" r:id="rId134" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/119/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E136" r:id="rId135" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/120/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E137" r:id="rId136" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/121/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E138" r:id="rId137" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/122/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E139" r:id="rId138" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/123/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E140" r:id="rId139" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/124/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E141" r:id="rId140" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/125/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E142" r:id="rId141" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/126/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E143" r:id="rId142" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/127/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E144" r:id="rId143" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/128/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E145" r:id="rId144" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/129/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E146" r:id="rId145" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/130/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E147" r:id="rId146" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/131/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E148" r:id="rId147" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/132/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E149" r:id="rId148" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/133/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E150" r:id="rId149" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/134/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E151" r:id="rId150" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/135/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E152" r:id="rId151" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/136/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E153" r:id="rId152" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/137/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E154" r:id="rId153" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/138/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E155" r:id="rId154" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/139/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E156" r:id="rId155" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/140/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E157" r:id="rId156" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/141/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E158" r:id="rId157" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/142/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E159" r:id="rId158" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/143/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E160" r:id="rId159" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/144/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E161" r:id="rId160" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/145/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E162" r:id="rId161" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/146/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E163" r:id="rId162" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/147/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E164" r:id="rId163" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/148/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E165" r:id="rId164" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/149/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E166" r:id="rId165" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/150/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E167" r:id="rId166" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/151/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E168" r:id="rId167" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/152/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E169" r:id="rId168" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/153/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E170" r:id="rId169" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/154/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E171" r:id="rId170" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/155/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E172" r:id="rId171" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/156/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E173" r:id="rId172" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/157/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E174" r:id="rId173" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/158/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E175" r:id="rId174" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/159/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E176" r:id="rId175" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/160/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E177" r:id="rId176" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/161/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E178" r:id="rId177" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/168/?_changelist_filters=all%3D%26o%3D2"/>
+    <hyperlink ref="E179" r:id="rId178" display="http://localhost:8000/appservice4/canka/basic_admin/CanKa/user/171/?_changelist_filters=all%3D%26o%3D2"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4625,10 +6901,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F8"/>
+  <dimension ref="A2:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4637,12 +6913,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="16" thickBot="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="22" thickBot="1">
       <c r="A3" s="2" t="s">
@@ -4744,6 +7020,91 @@
         <v>19948</v>
       </c>
       <c r="E8" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="19">
+        <v>20160119</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="19">
+        <v>14954</v>
+      </c>
+      <c r="E9" s="19">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="19">
+        <v>20160122</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="19">
+        <v>4956</v>
+      </c>
+      <c r="E10" s="19">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="19">
+        <v>20160126</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="19">
+        <v>3957</v>
+      </c>
+      <c r="E11" s="19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="19">
+        <v>20160127</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="19">
+        <v>-502.8</v>
+      </c>
+      <c r="E12" s="19">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="19">
+        <v>20160202</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="19">
+        <v>9496.7999999999993</v>
+      </c>
+      <c r="E13" s="19">
         <v>1</v>
       </c>
     </row>

</xml_diff>